<commit_message>
published all changes, commented
</commit_message>
<xml_diff>
--- a/Product Data per State.xlsx
+++ b/Product Data per State.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/OR8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DFD41FE2-6EA3-4369-AD56-4619602AEBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1401422D-65AE-4A4E-ADD1-E1C2F9EE870A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{DFD41FE2-6EA3-4369-AD56-4619602AEBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA420EA-7C7B-4CD3-AD36-A18B5FFAC652}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF9D25FB-F42D-42BB-A768-4008AE9B880C}"/>
   </bookViews>
@@ -322,6 +322,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,12 +648,14 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.7265625" style="3"/>
     <col min="5" max="5" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
@@ -698,34 +704,34 @@
         <v>11</v>
       </c>
       <c r="B2" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>3</v>
-      </c>
       <c r="G2" s="3">
-        <v>543</v>
+        <v>207</v>
       </c>
       <c r="H2" s="3">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3">
-        <v>728</v>
+        <v>453</v>
       </c>
       <c r="J2" s="3">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3">
-        <v>9765</v>
+        <v>9365</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -733,34 +739,34 @@
         <v>12</v>
       </c>
       <c r="B3" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3">
-        <v>2365</v>
+        <v>2029</v>
       </c>
       <c r="H3" s="3">
-        <v>509</v>
+        <v>29</v>
       </c>
       <c r="I3" s="3">
-        <v>3929</v>
+        <v>3654</v>
       </c>
       <c r="J3" s="3">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="K3" s="3">
-        <v>67976</v>
+        <v>67576</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -768,34 +774,34 @@
         <v>13</v>
       </c>
       <c r="B4" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3">
-        <v>1294</v>
+        <v>958</v>
       </c>
       <c r="H4" s="3">
-        <v>306</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3">
-        <v>2419</v>
+        <v>2144</v>
       </c>
       <c r="J4" s="3">
-        <v>153</v>
+        <v>33</v>
       </c>
       <c r="K4" s="3">
-        <v>40665</v>
+        <v>40265</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -803,34 +809,34 @@
         <v>14</v>
       </c>
       <c r="B5" s="3">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G5" s="3">
-        <v>3413</v>
+        <v>3077</v>
       </c>
       <c r="H5" s="3">
-        <v>261</v>
+        <v>0</v>
       </c>
       <c r="I5" s="3">
-        <v>5868</v>
+        <v>5593</v>
       </c>
       <c r="J5" s="3">
-        <v>250</v>
+        <v>130</v>
       </c>
       <c r="K5" s="3">
-        <v>98705</v>
+        <v>98305</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -838,34 +844,34 @@
         <v>15</v>
       </c>
       <c r="B6" s="3">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C6" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E6" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G6" s="3">
-        <v>16316</v>
+        <v>15980</v>
       </c>
       <c r="H6" s="3">
-        <v>1004</v>
+        <v>524</v>
       </c>
       <c r="I6" s="3">
-        <v>29994</v>
+        <v>29719</v>
       </c>
       <c r="J6" s="3">
-        <v>742</v>
+        <v>622</v>
       </c>
       <c r="K6" s="3">
-        <v>516565</v>
+        <v>516165</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -873,34 +879,34 @@
         <v>16</v>
       </c>
       <c r="B7" s="3">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2360</v>
+      </c>
+      <c r="H7" s="3">
+        <v>106</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4471</v>
+      </c>
+      <c r="J7" s="3">
         <v>53</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>36</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2696</v>
-      </c>
-      <c r="H7" s="3">
-        <v>586</v>
-      </c>
-      <c r="I7" s="3">
-        <v>4746</v>
-      </c>
-      <c r="J7" s="3">
-        <v>173</v>
-      </c>
       <c r="K7" s="3">
-        <v>77876</v>
+        <v>77476</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -908,34 +914,34 @@
         <v>17</v>
       </c>
       <c r="B8" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3">
-        <v>1531</v>
+        <v>1195</v>
       </c>
       <c r="H8" s="3">
-        <v>361</v>
+        <v>0</v>
       </c>
       <c r="I8" s="3">
-        <v>2963</v>
+        <v>2688</v>
       </c>
       <c r="J8" s="3">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="K8" s="3">
-        <v>48080</v>
+        <v>47680</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -943,34 +949,34 @@
         <v>18</v>
       </c>
       <c r="B9" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
-        <v>353</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3">
-        <v>592</v>
+        <v>317</v>
       </c>
       <c r="J9" s="3">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>9351</v>
+        <v>8951</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -978,34 +984,34 @@
         <v>19</v>
       </c>
       <c r="B10" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" s="3">
-        <v>576</v>
+        <v>240</v>
       </c>
       <c r="H10" s="3">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
-        <v>921</v>
+        <v>646</v>
       </c>
       <c r="J10" s="3">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="K10" s="3">
-        <v>13828</v>
+        <v>13428</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1013,34 +1019,34 @@
         <v>20</v>
       </c>
       <c r="B11" s="3">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C11" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E11" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="3">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G11" s="3">
-        <v>9663</v>
+        <v>9327</v>
       </c>
       <c r="H11" s="3">
-        <v>814</v>
+        <v>334</v>
       </c>
       <c r="I11" s="3">
-        <v>17567</v>
+        <v>17292</v>
       </c>
       <c r="J11" s="3">
-        <v>527</v>
+        <v>407</v>
       </c>
       <c r="K11" s="3">
-        <v>299651</v>
+        <v>299251</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -1048,34 +1054,34 @@
         <v>21</v>
       </c>
       <c r="B12" s="3">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E12" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F12" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G12" s="3">
-        <v>4876</v>
+        <v>4540</v>
       </c>
       <c r="H12" s="3">
-        <v>619</v>
+        <v>139</v>
       </c>
       <c r="I12" s="3">
-        <v>8508</v>
+        <v>8233</v>
       </c>
       <c r="J12" s="3">
-        <v>310</v>
+        <v>190</v>
       </c>
       <c r="K12" s="3">
-        <v>146497</v>
+        <v>146097</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1083,34 +1089,34 @@
         <v>22</v>
       </c>
       <c r="B13" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13" s="3">
-        <v>639</v>
+        <v>303</v>
       </c>
       <c r="H13" s="3">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="I13" s="3">
-        <v>1101</v>
+        <v>826</v>
       </c>
       <c r="J13" s="3">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="K13" s="3">
-        <v>19057</v>
+        <v>18657</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1118,34 +1124,34 @@
         <v>23</v>
       </c>
       <c r="B14" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3">
-        <v>1444</v>
+        <v>1108</v>
       </c>
       <c r="H14" s="3">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="I14" s="3">
-        <v>2491</v>
+        <v>2216</v>
       </c>
       <c r="J14" s="3">
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="K14" s="3">
-        <v>42748</v>
+        <v>42348</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1153,34 +1159,34 @@
         <v>24</v>
       </c>
       <c r="B15" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="3">
-        <v>1142</v>
+        <v>806</v>
       </c>
       <c r="H15" s="3">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3">
-        <v>1596</v>
+        <v>1321</v>
       </c>
       <c r="J15" s="3">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="K15" s="3">
-        <v>26174</v>
+        <v>25774</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1188,34 +1194,34 @@
         <v>25</v>
       </c>
       <c r="B16" s="3">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C16" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E16" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G16" s="3">
-        <v>5476</v>
+        <v>5140</v>
       </c>
       <c r="H16" s="3">
-        <v>771</v>
+        <v>291</v>
       </c>
       <c r="I16" s="3">
-        <v>9822</v>
+        <v>9547</v>
       </c>
       <c r="J16" s="3">
-        <v>265</v>
+        <v>145</v>
       </c>
       <c r="K16" s="3">
-        <v>166429</v>
+        <v>166029</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -1223,34 +1229,34 @@
         <v>26</v>
       </c>
       <c r="B17" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G17" s="3">
-        <v>3107</v>
+        <v>2771</v>
       </c>
       <c r="H17" s="3">
-        <v>204</v>
+        <v>0</v>
       </c>
       <c r="I17" s="3">
-        <v>5274</v>
+        <v>4999</v>
       </c>
       <c r="J17" s="3">
-        <v>222</v>
+        <v>102</v>
       </c>
       <c r="K17" s="3">
-        <v>90996</v>
+        <v>90596</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1258,34 +1264,34 @@
         <v>27</v>
       </c>
       <c r="B18" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" s="3">
-        <v>1522</v>
+        <v>1186</v>
       </c>
       <c r="H18" s="3">
-        <v>293</v>
+        <v>0</v>
       </c>
       <c r="I18" s="3">
-        <v>2377</v>
+        <v>2102</v>
       </c>
       <c r="J18" s="3">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="K18" s="3">
-        <v>39164</v>
+        <v>38764</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1293,34 +1299,34 @@
         <v>28</v>
       </c>
       <c r="B19" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3">
-        <v>2014</v>
+        <v>1678</v>
       </c>
       <c r="H19" s="3">
-        <v>451</v>
+        <v>0</v>
       </c>
       <c r="I19" s="3">
-        <v>3578</v>
+        <v>3303</v>
       </c>
       <c r="J19" s="3">
-        <v>106</v>
+        <v>0</v>
       </c>
       <c r="K19" s="3">
-        <v>60070</v>
+        <v>59670</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
@@ -1328,34 +1334,34 @@
         <v>29</v>
       </c>
       <c r="B20" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3">
-        <v>2180</v>
+        <v>1844</v>
       </c>
       <c r="H20" s="3">
-        <v>456</v>
+        <v>0</v>
       </c>
       <c r="I20" s="3">
-        <v>3697</v>
+        <v>3422</v>
       </c>
       <c r="J20" s="3">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="K20" s="3">
-        <v>60782</v>
+        <v>60382</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -1363,34 +1369,34 @@
         <v>30</v>
       </c>
       <c r="B21" s="3">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G21" s="3">
-        <v>2921</v>
+        <v>2585</v>
       </c>
       <c r="H21" s="3">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="I21" s="3">
-        <v>5621</v>
+        <v>5346</v>
       </c>
       <c r="J21" s="3">
-        <v>229</v>
+        <v>109</v>
       </c>
       <c r="K21" s="3">
-        <v>93077</v>
+        <v>92677</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -1398,34 +1404,34 @@
         <v>31</v>
       </c>
       <c r="B22" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E22" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G22" s="3">
-        <v>2744</v>
+        <v>2408</v>
       </c>
       <c r="H22" s="3">
-        <v>616</v>
+        <v>136</v>
       </c>
       <c r="I22" s="3">
-        <v>4950</v>
+        <v>4675</v>
       </c>
       <c r="J22" s="3">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="K22" s="3">
-        <v>82000</v>
+        <v>81600</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
@@ -1433,34 +1439,34 @@
         <v>32</v>
       </c>
       <c r="B23" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" s="3">
-        <v>837</v>
+        <v>501</v>
       </c>
       <c r="H23" s="3">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="I23" s="3">
-        <v>1278</v>
+        <v>1003</v>
       </c>
       <c r="J23" s="3">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="K23" s="3">
-        <v>18867</v>
+        <v>18467</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -1468,34 +1474,34 @@
         <v>33</v>
       </c>
       <c r="B24" s="3">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="3">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G24" s="3">
-        <v>4439</v>
+        <v>4103</v>
       </c>
       <c r="H24" s="3">
-        <v>520</v>
+        <v>40</v>
       </c>
       <c r="I24" s="3">
-        <v>7686</v>
+        <v>7411</v>
       </c>
       <c r="J24" s="3">
-        <v>260</v>
+        <v>140</v>
       </c>
       <c r="K24" s="3">
-        <v>133266</v>
+        <v>132866</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
@@ -1503,34 +1509,34 @@
         <v>34</v>
       </c>
       <c r="B25" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G25" s="3">
-        <v>2545</v>
+        <v>2209</v>
       </c>
       <c r="H25" s="3">
-        <v>572</v>
+        <v>92</v>
       </c>
       <c r="I25" s="3">
-        <v>4398</v>
+        <v>4123</v>
       </c>
       <c r="J25" s="3">
-        <v>166</v>
+        <v>46</v>
       </c>
       <c r="K25" s="3">
-        <v>76187</v>
+        <v>75787</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
@@ -1538,34 +1544,34 @@
         <v>35</v>
       </c>
       <c r="B26" s="3">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G26" s="3">
-        <v>2800</v>
+        <v>2464</v>
       </c>
       <c r="H26" s="3">
-        <v>618</v>
+        <v>138</v>
       </c>
       <c r="I26" s="3">
-        <v>4990</v>
+        <v>4715</v>
       </c>
       <c r="J26" s="3">
-        <v>189</v>
+        <v>69</v>
       </c>
       <c r="K26" s="3">
-        <v>82238</v>
+        <v>81838</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
@@ -1573,34 +1579,34 @@
         <v>36</v>
       </c>
       <c r="B27" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G27" s="3">
-        <v>1519</v>
+        <v>1183</v>
       </c>
       <c r="H27" s="3">
-        <v>293</v>
+        <v>0</v>
       </c>
       <c r="I27" s="3">
-        <v>2375</v>
+        <v>2100</v>
       </c>
       <c r="J27" s="3">
-        <v>147</v>
+        <v>27</v>
       </c>
       <c r="K27" s="3">
-        <v>39151</v>
+        <v>38751</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -1608,34 +1614,34 @@
         <v>37</v>
       </c>
       <c r="B28" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F28" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G28" s="3">
-        <v>592</v>
+        <v>256</v>
       </c>
       <c r="H28" s="3">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="I28" s="3">
-        <v>898</v>
+        <v>623</v>
       </c>
       <c r="J28" s="3">
-        <v>8512</v>
+        <v>8392</v>
       </c>
       <c r="K28" s="3">
-        <v>15337</v>
+        <v>14937</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1643,34 +1649,34 @@
         <v>38</v>
       </c>
       <c r="B29" s="3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="3">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E29" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G29" s="3">
-        <v>4536</v>
+        <v>4200</v>
       </c>
       <c r="H29" s="3">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="I29" s="3">
-        <v>8300</v>
+        <v>8025</v>
       </c>
       <c r="J29" s="3">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="K29" s="3">
-        <v>143601</v>
+        <v>143201</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -1678,34 +1684,34 @@
         <v>39</v>
       </c>
       <c r="B30" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
         <v>4</v>
       </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>3</v>
-      </c>
       <c r="G30" s="3">
-        <v>383</v>
+        <v>47</v>
       </c>
       <c r="H30" s="3">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="I30" s="3">
-        <v>853</v>
+        <v>578</v>
       </c>
       <c r="J30" s="3">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="K30" s="3">
-        <v>10520</v>
+        <v>10120</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -1713,34 +1719,34 @@
         <v>40</v>
       </c>
       <c r="B31" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31" s="3">
-        <v>854</v>
+        <v>518</v>
       </c>
       <c r="H31" s="3">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="I31" s="3">
-        <v>1630</v>
+        <v>1355</v>
       </c>
       <c r="J31" s="3">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="K31" s="3">
-        <v>26379</v>
+        <v>25979</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -1748,34 +1754,34 @@
         <v>41</v>
       </c>
       <c r="B32" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E32" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G32" s="3">
-        <v>859</v>
+        <v>523</v>
       </c>
       <c r="H32" s="3">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="I32" s="3">
-        <v>1294</v>
+        <v>1019</v>
       </c>
       <c r="J32" s="3">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="K32" s="3">
-        <v>18962</v>
+        <v>18562</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
@@ -1783,34 +1789,34 @@
         <v>42</v>
       </c>
       <c r="B33" s="3">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C33" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="3">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F33" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G33" s="3">
-        <v>3852</v>
+        <v>3516</v>
       </c>
       <c r="H33" s="3">
-        <v>446</v>
+        <v>0</v>
       </c>
       <c r="I33" s="3">
-        <v>7201</v>
+        <v>6926</v>
       </c>
       <c r="J33" s="3">
-        <v>223</v>
+        <v>103</v>
       </c>
       <c r="K33" s="3">
-        <v>123307</v>
+        <v>122907</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
@@ -1818,34 +1824,34 @@
         <v>43</v>
       </c>
       <c r="B34" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G34" s="3">
-        <v>992</v>
+        <v>656</v>
       </c>
       <c r="H34" s="3">
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="I34" s="3">
-        <v>1694</v>
+        <v>1419</v>
       </c>
       <c r="J34" s="3">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="K34" s="3">
-        <v>28412</v>
+        <v>28012</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -1853,34 +1859,34 @@
         <v>44</v>
       </c>
       <c r="B35" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="3">
-        <v>1399</v>
+        <v>1063</v>
       </c>
       <c r="H35" s="3">
-        <v>318</v>
+        <v>0</v>
       </c>
       <c r="I35" s="3">
-        <v>2459</v>
+        <v>2184</v>
       </c>
       <c r="J35" s="3">
-        <v>159</v>
+        <v>39</v>
       </c>
       <c r="K35" s="3">
-        <v>42556</v>
+        <v>42156</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -1888,34 +1894,34 @@
         <v>45</v>
       </c>
       <c r="B36" s="3">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C36" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="3">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E36" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F36" s="3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G36" s="3">
-        <v>8131</v>
+        <v>7795</v>
       </c>
       <c r="H36" s="3">
-        <v>511</v>
+        <v>31</v>
       </c>
       <c r="I36" s="3">
-        <v>15218</v>
+        <v>14943</v>
       </c>
       <c r="J36" s="3">
-        <v>375</v>
+        <v>255</v>
       </c>
       <c r="K36" s="3">
-        <v>259408</v>
+        <v>259008</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -1923,34 +1929,34 @@
         <v>46</v>
       </c>
       <c r="B37" s="3">
+        <v>108</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>74</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>51</v>
+      </c>
+      <c r="G37" s="3">
+        <v>4828</v>
+      </c>
+      <c r="H37" s="3">
+        <v>215</v>
+      </c>
+      <c r="I37" s="3">
+        <v>9018</v>
+      </c>
+      <c r="J37" s="3">
         <v>107</v>
       </c>
-      <c r="C37" s="3">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3">
-        <v>73</v>
-      </c>
-      <c r="E37" s="3">
-        <v>3</v>
-      </c>
-      <c r="F37" s="3">
-        <v>50</v>
-      </c>
-      <c r="G37" s="3">
-        <v>5164</v>
-      </c>
-      <c r="H37" s="3">
-        <v>695</v>
-      </c>
-      <c r="I37" s="3">
-        <v>9293</v>
-      </c>
-      <c r="J37" s="3">
-        <v>227</v>
-      </c>
       <c r="K37" s="3">
-        <v>156211</v>
+        <v>155811</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -1958,34 +1964,34 @@
         <v>47</v>
       </c>
       <c r="B38" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E38" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F38" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G38" s="3">
-        <v>1710</v>
+        <v>1374</v>
       </c>
       <c r="H38" s="3">
-        <v>404</v>
+        <v>0</v>
       </c>
       <c r="I38" s="3">
-        <v>3226</v>
+        <v>2951</v>
       </c>
       <c r="J38" s="3">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="K38" s="3">
-        <v>53808</v>
+        <v>53408</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
@@ -1993,34 +1999,34 @@
         <v>48</v>
       </c>
       <c r="B39" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G39" s="3">
-        <v>2000</v>
+        <v>1664</v>
       </c>
       <c r="H39" s="3">
-        <v>422</v>
+        <v>0</v>
       </c>
       <c r="I39" s="3">
-        <v>3399</v>
+        <v>3124</v>
       </c>
       <c r="J39" s="3">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="K39" s="3">
-        <v>56093</v>
+        <v>55693</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -2028,34 +2034,34 @@
         <v>49</v>
       </c>
       <c r="B40" s="3">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" s="3">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E40" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F40" s="3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G40" s="3">
-        <v>5569</v>
+        <v>5233</v>
       </c>
       <c r="H40" s="3">
-        <v>332</v>
+        <v>0</v>
       </c>
       <c r="I40" s="3">
-        <v>10023</v>
+        <v>9748</v>
       </c>
       <c r="J40" s="3">
-        <v>286</v>
+        <v>166</v>
       </c>
       <c r="K40" s="3">
-        <v>171789</v>
+        <v>171389</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
@@ -2063,34 +2069,34 @@
         <v>50</v>
       </c>
       <c r="B41" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E41" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G41" s="3">
-        <v>463</v>
+        <v>127</v>
       </c>
       <c r="H41" s="3">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="I41" s="3">
-        <v>1081</v>
+        <v>806</v>
       </c>
       <c r="J41" s="3">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="K41" s="3">
-        <v>14786</v>
+        <v>14386</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
@@ -2098,34 +2104,34 @@
         <v>51</v>
       </c>
       <c r="B42" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E42" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F42" s="3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G42" s="3">
-        <v>2282</v>
+        <v>1946</v>
       </c>
       <c r="H42" s="3">
-        <v>536</v>
+        <v>56</v>
       </c>
       <c r="I42" s="3">
-        <v>4315</v>
+        <v>4040</v>
       </c>
       <c r="J42" s="3">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="K42" s="3">
-        <v>71540</v>
+        <v>71140</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
@@ -2133,34 +2139,34 @@
         <v>52</v>
       </c>
       <c r="B43" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43" s="3">
-        <v>519</v>
+        <v>183</v>
       </c>
       <c r="H43" s="3">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="I43" s="3">
-        <v>916</v>
+        <v>641</v>
       </c>
       <c r="J43" s="3">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="K43" s="3">
-        <v>12545</v>
+        <v>12145</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
@@ -2168,34 +2174,34 @@
         <v>53</v>
       </c>
       <c r="B44" s="3">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G44" s="3">
-        <v>3021</v>
+        <v>2685</v>
       </c>
       <c r="H44" s="3">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="I44" s="3">
-        <v>5658</v>
+        <v>5383</v>
       </c>
       <c r="J44" s="3">
-        <v>235</v>
+        <v>115</v>
       </c>
       <c r="K44" s="3">
-        <v>94548</v>
+        <v>94148</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
@@ -2203,34 +2209,34 @@
         <v>54</v>
       </c>
       <c r="B45" s="3">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C45" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D45" s="3">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E45" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F45" s="3">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G45" s="3">
-        <v>12668</v>
+        <v>12332</v>
       </c>
       <c r="H45" s="3">
-        <v>1120</v>
+        <v>640</v>
       </c>
       <c r="I45" s="3">
-        <v>23484</v>
+        <v>23209</v>
       </c>
       <c r="J45" s="3">
-        <v>680</v>
+        <v>560</v>
       </c>
       <c r="K45" s="3">
-        <v>404452</v>
+        <v>404052</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
@@ -2238,34 +2244,34 @@
         <v>55</v>
       </c>
       <c r="B46" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G46" s="3">
-        <v>1507</v>
+        <v>1171</v>
       </c>
       <c r="H46" s="3">
-        <v>341</v>
+        <v>0</v>
       </c>
       <c r="I46" s="3">
-        <v>2741</v>
+        <v>2466</v>
       </c>
       <c r="J46" s="3">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="K46" s="3">
-        <v>45498</v>
+        <v>45098</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
@@ -2273,34 +2279,34 @@
         <v>56</v>
       </c>
       <c r="B47" s="3">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C47" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E47" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G47" s="3">
-        <v>3861</v>
+        <v>3525</v>
       </c>
       <c r="H47" s="3">
-        <v>389</v>
+        <v>0</v>
       </c>
       <c r="I47" s="3">
-        <v>6868</v>
+        <v>6593</v>
       </c>
       <c r="J47" s="3">
-        <v>194</v>
+        <v>74</v>
       </c>
       <c r="K47" s="3">
-        <v>115508</v>
+        <v>115108</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
@@ -2308,34 +2314,34 @@
         <v>57</v>
       </c>
       <c r="B48" s="3">
+        <v>6</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3">
         <v>5</v>
       </c>
-      <c r="C48" s="3">
-        <v>0</v>
-      </c>
-      <c r="D48" s="3">
-        <v>4</v>
-      </c>
       <c r="E48" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G48" s="3">
-        <v>579</v>
+        <v>243</v>
       </c>
       <c r="H48" s="3">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="I48" s="3">
-        <v>513</v>
+        <v>238</v>
       </c>
       <c r="J48" s="3">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K48" s="3">
-        <v>8880</v>
+        <v>8480</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
@@ -2343,34 +2349,34 @@
         <v>58</v>
       </c>
       <c r="B49" s="3">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" s="3">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E49" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" s="3">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G49" s="3">
-        <v>3400</v>
+        <v>3064</v>
       </c>
       <c r="H49" s="3">
-        <v>299</v>
+        <v>0</v>
       </c>
       <c r="I49" s="3">
-        <v>5993</v>
+        <v>5718</v>
       </c>
       <c r="J49" s="3">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="K49" s="3">
-        <v>103610</v>
+        <v>103210</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
@@ -2378,34 +2384,34 @@
         <v>59</v>
       </c>
       <c r="B50" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C50" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E50" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F50" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G50" s="3">
-        <v>2477</v>
+        <v>2141</v>
       </c>
       <c r="H50" s="3">
-        <v>589</v>
+        <v>109</v>
       </c>
       <c r="I50" s="3">
-        <v>4554</v>
+        <v>4279</v>
       </c>
       <c r="J50" s="3">
-        <v>175</v>
+        <v>55</v>
       </c>
       <c r="K50" s="3">
-        <v>78374</v>
+        <v>77974</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
@@ -2413,34 +2419,34 @@
         <v>60</v>
       </c>
       <c r="B51" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G51" s="3">
-        <v>799</v>
+        <v>463</v>
       </c>
       <c r="H51" s="3">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="I51" s="3">
-        <v>1386</v>
+        <v>1111</v>
       </c>
       <c r="J51" s="3">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="K51" s="3">
-        <v>23664</v>
+        <v>23264</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
@@ -2448,34 +2454,34 @@
         <v>61</v>
       </c>
       <c r="B52" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="3">
+        <v>4</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
         <v>3</v>
       </c>
-      <c r="E52" s="3">
-        <v>0</v>
-      </c>
-      <c r="F52" s="3">
-        <v>2</v>
-      </c>
       <c r="G52" s="3">
-        <v>358</v>
+        <v>22</v>
       </c>
       <c r="H52" s="3">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="I52" s="3">
-        <v>630</v>
+        <v>355</v>
       </c>
       <c r="J52" s="3">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="K52" s="3">
-        <v>7932</v>
+        <v>7532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>